<commit_message>
made dynamic selection for title and state of issue dropdown
</commit_message>
<xml_diff>
--- a/sales-e2e/resources/Reprice_Data/Estimated_Cost_Test_Data.xlsx
+++ b/sales-e2e/resources/Reprice_Data/Estimated_Cost_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravipandey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravipandey/Desktop/Savages Testcafe E2E Test/sales-e2e/sales-e2e/resources/Reprice_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC9BEAA-133A-C04E-ACB6-4532BADAC6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0296F55F-4BD5-E14F-A87C-94B1504691FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{7D8B3CEE-CBCB-4847-B6D7-D43D76C10306}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{7D8B3CEE-CBCB-4847-B6D7-D43D76C10306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -735,7 +735,7 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <v>1477.8053103</v>
+        <v>1477.2053103000001</v>
       </c>
       <c r="J24" s="2">
         <v>0</v>

</xml_diff>